<commit_message>
Added Spanish translation (by https://twitter.com/voces25)
</commit_message>
<xml_diff>
--- a/10-basic-facts-for-human-and-planetary-survival.xlsx
+++ b/10-basic-facts-for-human-and-planetary-survival.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Parents_For_Future\Github\parents4future\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565BD690-D3C3-4B73-85FB-EB9DA1B5B152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA60C31-468B-45E6-BD1F-45CF04B70281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{D0F2AC70-04F0-4F0C-9676-9D76491B6638}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{D0F2AC70-04F0-4F0C-9676-9D76491B6638}"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
     <sheet name="German" sheetId="2" r:id="rId2"/>
+    <sheet name="Spanish" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>➀</t>
   </si>
@@ -208,13 +209,84 @@
   </si>
   <si>
     <t>https://twitter.com/parents4future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 hechos básicos para la supervivencia humana y planetaria   </t>
+  </si>
+  <si>
+    <t>Esfera física, natural y tecnológica</t>
+  </si>
+  <si>
+    <t>Esfera social, económica, cultural y política</t>
+  </si>
+  <si>
+    <t>Diagnóstico</t>
+  </si>
+  <si>
+    <t>Pronóstico</t>
+  </si>
+  <si>
+    <t>Prevención</t>
+  </si>
+  <si>
+    <t>Intervención</t>
+  </si>
+  <si>
+    <t>Panorama</t>
+  </si>
+  <si>
+    <t>Las crisis climáticas y ecológicas
+son malas, muy malas.</t>
+  </si>
+  <si>
+    <t>Vista la trayectoria actual, las crisis climáticas serán muchísimo peor que ahora</t>
+  </si>
+  <si>
+    <t>Todavía estamos a tiempo de 
+prevenir el empeoramiento de esta 
+gran crisis climática y ecológica</t>
+  </si>
+  <si>
+    <t>Esto va a requerir un cambio radical:
+reducir la escala de consumo.</t>
+  </si>
+  <si>
+    <t>Este cambio radical es compatible
+con el bienestar humano universal
+y unas sociedades más sanas.</t>
+  </si>
+  <si>
+    <t>Nuestras economías y gobiernos son responsables de estas crisis y de que se mantengan en el tiempo.</t>
+  </si>
+  <si>
+    <t>Nosotros, el pueblo, tenemos el poder de convertirnos en una contra-fuerza necesaria a las industrias de combustibles fósiles y su sistemática corrupción.</t>
+  </si>
+  <si>
+    <t>Tenemos que hacerlo nosotros mismos, trabajando juntos.
+Nadie más nos salvará. Nosotros somos lo que se interpone entre nuestro mundo y su destrucción.</t>
+  </si>
+  <si>
+    <t>Como activistas comprometidos, construiremos
+sociedades resilientes, equitativas y justas,
+dentro de los límites planetarios.</t>
+  </si>
+  <si>
+    <t>Nos tememos que los 
+poderes económicos mantengan 
+la desastrosa trayectoria climática actual</t>
+  </si>
+  <si>
+    <t>https://twitter.com/voces25</t>
+  </si>
+  <si>
+    <t>Spanish:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +394,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="21">
     <fill>
@@ -458,7 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -490,42 +576,6 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -564,6 +614,51 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="20" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -896,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53DA77D2-ED38-4D0B-A1F9-852B3763769A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -910,154 +1005,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="27"/>
     </row>
     <row r="3" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="6" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="30"/>
     </row>
     <row r="8" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="12"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="30"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="12"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="30"/>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="34" t="s">
+    <row r="13" spans="1:4" s="21" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
     </row>
     <row r="14" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A11:D11"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A11:D11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" xr:uid="{58A0D118-A586-46E2-ACAC-F34029EF2FB8}"/>
@@ -1072,7 +1167,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1085,144 +1180,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="27"/>
     </row>
     <row r="3" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="6" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="30"/>
     </row>
     <row r="8" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="12"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="30"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="17" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="12"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="30"/>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="34" t="s">
+    <row r="13" spans="1:4" s="21" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="23" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1245,4 +1340,184 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6E1697-54FE-4CD8-BE64-CDF1D91CF19F}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="5.796875" customWidth="1"/>
+    <col min="2" max="2" width="50.59765625" customWidth="1"/>
+    <col min="3" max="3" width="5.796875" customWidth="1"/>
+    <col min="4" max="4" width="50.59765625" customWidth="1"/>
+    <col min="6" max="6" width="11.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="27"/>
+    </row>
+    <row r="3" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="30"/>
+    </row>
+    <row r="6" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="30"/>
+    </row>
+    <row r="8" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="35"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="30"/>
+    </row>
+    <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="21" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{15EF1A98-3617-480B-AAB9-CF98D58FD34F}"/>
+    <hyperlink ref="D13" r:id="rId2" xr:uid="{280213BF-1BEF-43D9-9E44-E79972A0386C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Swedish translation (by https://twitter.com/scepterfilm)
</commit_message>
<xml_diff>
--- a/10-basic-facts-for-human-and-planetary-survival.xlsx
+++ b/10-basic-facts-for-human-and-planetary-survival.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Parents_For_Future\Github\parents4future\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA60C31-468B-45E6-BD1F-45CF04B70281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49951B5-539D-4319-B6DB-268B82BC81F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{D0F2AC70-04F0-4F0C-9676-9D76491B6638}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15481" xr2:uid="{D0F2AC70-04F0-4F0C-9676-9D76491B6638}"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
     <sheet name="German" sheetId="2" r:id="rId2"/>
     <sheet name="Spanish" sheetId="3" r:id="rId3"/>
+    <sheet name="Swedish" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
   <si>
     <t>➀</t>
   </si>
@@ -280,6 +281,79 @@
   </si>
   <si>
     <t>Spanish:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 grundläggande fakta för mänsklig och planetär överlevnad         </t>
+  </si>
+  <si>
+    <t>Fysisk, naturlig och teknisk sfär</t>
+  </si>
+  <si>
+    <t>Social, ekonomisk, kulturell och politisk sfär</t>
+  </si>
+  <si>
+    <t>Diagnos</t>
+  </si>
+  <si>
+    <t>Kriserna för klimatet och den biologiska mångfalden är mycket allvarliga.</t>
+  </si>
+  <si>
+    <t>Våra regeringar och ekonomiska system är ansvariga för och förvärrar dessa kriser.</t>
+  </si>
+  <si>
+    <t>Prognos</t>
+  </si>
+  <si>
+    <t>Om vi fortsätter som vi gör nu
+kommer det att bli mycket värre.</t>
+  </si>
+  <si>
+    <t>Vi bör förvänta oss att ekonomiskt
+starka krafter kommer försöka hålla fast
+vid vår nuvarande katastrofala kurs.</t>
+  </si>
+  <si>
+    <t>Förebyggande</t>
+  </si>
+  <si>
+    <t>Vi kan fortfarande, just nu, 
+förhindra att kriserna förvärras.</t>
+  </si>
+  <si>
+    <t>Vi, folket, har makten att vara en
+nödvändig motkraft till fossilindustrin
+och dess korruption.</t>
+  </si>
+  <si>
+    <t>Åtgärder</t>
+  </si>
+  <si>
+    <t>Detta kräver radikala förändringar och
+minskning av konsumtionen.</t>
+  </si>
+  <si>
+    <t>Vi måste göra detta själva och arbeta
+tillsammans. Ingen annan
+kommer att rädda oss.</t>
+  </si>
+  <si>
+    <t>Utsikt</t>
+  </si>
+  <si>
+    <t>Dessa radikala förändringar är förenliga med 
+universellt mänskligt välbefinnande 
+och hälsosammare samhällen.</t>
+  </si>
+  <si>
+    <t>Som engagerade aktivister kommer vi att 
+bygga motståndskraftiga, jämlika och
+rättvisa samhällen inom planetens gränser.</t>
+  </si>
+  <si>
+    <t>https://twitter.com/scepterfilm</t>
+  </si>
+  <si>
+    <t>Swedish:</t>
   </si>
 </sst>
 </file>
@@ -615,42 +689,6 @@
     <xf numFmtId="0" fontId="13" fillId="20" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -659,6 +697,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -991,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53DA77D2-ED38-4D0B-A1F9-852B3763769A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1005,30 +1079,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="35"/>
     </row>
     <row r="3" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
@@ -1045,12 +1119,12 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="30"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
@@ -1067,12 +1141,12 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="30"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -1089,12 +1163,12 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
@@ -1111,12 +1185,12 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
@@ -1145,14 +1219,14 @@
     <row r="14" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A5:D5"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" xr:uid="{58A0D118-A586-46E2-ACAC-F34029EF2FB8}"/>
@@ -1166,7 +1240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5FCAC5-DCBF-4292-9845-BB42D4861F7F}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -1180,30 +1254,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="35"/>
     </row>
     <row r="3" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
@@ -1220,12 +1294,12 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="30"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
@@ -1242,12 +1316,12 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="30"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -1264,12 +1338,12 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
@@ -1286,12 +1360,12 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
@@ -1346,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6E1697-54FE-4CD8-BE64-CDF1D91CF19F}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1360,30 +1434,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="35"/>
     </row>
     <row r="3" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
@@ -1395,17 +1469,17 @@
       <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="24" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="30"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
@@ -1422,12 +1496,12 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="30"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -1439,17 +1513,17 @@
       <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="25" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
@@ -1461,17 +1535,17 @@
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
@@ -1520,4 +1594,184 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FFE970-342F-4AD6-86FB-24E1A9E00BFE}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="5.796875" customWidth="1"/>
+    <col min="2" max="2" width="50.59765625" customWidth="1"/>
+    <col min="3" max="3" width="5.796875" customWidth="1"/>
+    <col min="4" max="4" width="50.59765625" customWidth="1"/>
+    <col min="6" max="6" width="11.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+    </row>
+    <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="29"/>
+    </row>
+    <row r="6" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
+    </row>
+    <row r="8" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
+    </row>
+    <row r="10" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="31"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
+    </row>
+    <row r="12" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="21" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{A3E99CF4-E2B9-4391-B685-BCFA1001D288}"/>
+    <hyperlink ref="D13" r:id="rId2" xr:uid="{1A7BD36C-535E-4488-BB1E-0868A8D5E8C0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>